<commit_message>
Change Id->Ids in library/Models/PaginationParameters
</commit_message>
<xml_diff>
--- a/src/Journal/ExerciseMuscles/ExerciseMuscles.xlsx
+++ b/src/Journal/ExerciseMuscles/ExerciseMuscles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thin\source\repos\cool-server\src\Databases\Journal\Tables\ExerciseMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF9471-F071-479F-A447-B285E2A654BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A100A2-3F2E-40FD-9FBB-EC0D7BCC1C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="189">
   <si>
     <t>Id</t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t xml:space="preserve">6e9d2f1b-3c4a-4a7c-b5e8-9f1d3e2a7b6c  </t>
-  </si>
-  <si>
-    <t>2405609c-9db8-441a-b03a-2bb9235a0026</t>
   </si>
   <si>
     <t>74f82514-4119-43f5-aeea-adfdb9c3b554</t>
@@ -612,7 +609,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,19 +1011,19 @@
   <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="58.44140625" customWidth="1"/>
-    <col min="2" max="2" width="48.5546875" customWidth="1"/>
-    <col min="3" max="3" width="41.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1054,7 +1051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1076,7 +1073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1087,7 +1084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1098,7 +1095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1109,7 +1106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1120,7 +1117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1142,7 +1139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1153,7 +1150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1164,7 +1161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1175,7 +1172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1186,7 +1183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1197,7 +1194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1208,7 +1205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1230,7 +1227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1241,7 +1238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1252,7 +1249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1263,7 +1260,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1274,7 +1271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1285,7 +1282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1296,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1307,7 +1304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1318,7 +1315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1329,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1351,7 +1348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1362,7 +1359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1373,7 +1370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1384,7 +1381,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1395,7 +1392,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -1406,7 +1403,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1417,7 +1414,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +1425,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -1439,7 +1436,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -1450,7 +1447,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -1461,7 +1458,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -1472,7 +1469,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -1483,7 +1480,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -1494,7 +1491,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -1505,7 +1502,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1527,7 +1524,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1538,7 +1535,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1549,7 +1546,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1560,7 +1557,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15">
       <c r="A49" t="s">
         <v>75</v>
       </c>
@@ -1568,741 +1565,741 @@
         <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B50" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="C50" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="4" t="s">
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="B51" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="4" t="s">
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B53" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="C53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="4" t="s">
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B54" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="C54" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C54" s="4" t="s">
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="B55" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="3" t="s">
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="B57" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B59" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="C59" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="B60" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="C60" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B61" t="s">
         <v>103</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="3" t="s">
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="B62" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C62" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="B63" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C66" s="3" t="s">
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="B67" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C67" s="3" t="s">
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="B68" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C68" s="3" t="s">
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="7" t="s">
+      <c r="B69" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
+        <v>121</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
+        <v>123</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="C74" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
         <v>129</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="B75" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="B76" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
         <v>132</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="B77" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>133</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="B78" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="C78" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
         <v>135</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="B79" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>136</v>
       </c>
-      <c r="B79" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="B80" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="C80" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="7" t="s">
+      <c r="B81" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B81" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
+      <c r="B82" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="C82" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>141</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B83" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
         <v>142</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="B84" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
         <v>143</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="B85" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="C85" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
         <v>145</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="B86" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
         <v>146</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="B87" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
         <v>147</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="B88" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="C88" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
         <v>149</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="B89" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
         <v>150</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="B90" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
         <v>151</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="B91" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="C91" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
         <v>153</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>154</v>
-      </c>
       <c r="B92" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
+        <v>154</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="C93" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C93" s="3" t="s">
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="B94" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
         <v>158</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="B95" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
         <v>159</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="B96" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="C96" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
         <v>161</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>162</v>
-      </c>
       <c r="B97" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
+        <v>162</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
         <v>163</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="B99" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>165</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
+        <v>166</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
         <v>167</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="B102" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3">
       <c r="A104" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
+        <v>172</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
+        <v>175</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
         <v>176</v>
       </c>
-      <c r="B108" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="B109" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
+        <v>179</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
+        <v>182</v>
+      </c>
+      <c r="B113" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
+        <v>184</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B114" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C114" s="3" t="s">
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="B115" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
         <v>187</v>
       </c>
-      <c r="B115" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="B116" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Fix ExerciseMuscles excel file
</commit_message>
<xml_diff>
--- a/src/Journal/ExerciseMuscles/ExerciseMuscles.xlsx
+++ b/src/Journal/ExerciseMuscles/ExerciseMuscles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thin\source\repos\cool-server\src\Databases\Journal\Tables\ExerciseMuscle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thin\source\repos\cool-server\src\Journal\ExerciseMuscles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A100A2-3F2E-40FD-9FBB-EC0D7BCC1C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467D4419-7000-4751-8844-E410A56A9E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="188">
   <si>
     <t>Id</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t xml:space="preserve">2a3c9e1d-5b4f-4e7a-a6c8-3d1b7c2f9e4a  </t>
-  </si>
-  <si>
-    <t>2405609c-9db8-441a-b03a-2bb9235a0027</t>
   </si>
   <si>
     <t>a5a834bf-6351-4d7d-bcd7-9aefec2e89ff</t>
@@ -609,7 +606,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1011,19 +1008,19 @@
   <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1051,7 +1048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1062,7 +1059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1084,7 +1081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1095,7 +1092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1106,7 +1103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1117,7 +1114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1128,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1139,7 +1136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1150,7 +1147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1161,7 +1158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1172,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1183,7 +1180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1194,7 +1191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1205,7 +1202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1216,7 +1213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1227,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1238,7 +1235,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1249,7 +1246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1260,7 +1257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1271,7 +1268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1282,7 +1279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1293,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1304,7 +1301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1315,7 +1312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1326,7 +1323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1337,7 +1334,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1348,7 +1345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1359,7 +1356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1370,7 +1367,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1381,7 +1378,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -1403,7 +1400,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -1425,7 +1422,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -1436,7 +1433,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -1447,7 +1444,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -1458,7 +1455,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -1469,7 +1466,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -1480,7 +1477,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -1502,7 +1499,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -1513,7 +1510,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1524,7 +1521,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1535,7 +1532,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1546,7 +1543,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1557,7 +1554,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>75</v>
       </c>
@@ -1568,7 +1565,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -1576,730 +1573,730 @@
         <v>78</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+      <c r="B51" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="4" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
+      <c r="B53" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="C53" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="4" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+      <c r="B54" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="C54" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="4" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
+      <c r="B55" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="3" t="s">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+      <c r="B57" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
+      <c r="B59" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="C59" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>99</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+      <c r="B60" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="C60" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>101</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+      <c r="B61" t="s">
         <v>102</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C61" s="3" t="s">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+      <c r="B62" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C62" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>106</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+      <c r="B63" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C66" s="3" t="s">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
+      <c r="B67" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C67" s="3" t="s">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+      <c r="B68" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C68" s="3" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="7" t="s">
+      <c r="B69" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>124</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>126</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="C74" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>128</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+      <c r="B75" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>129</v>
       </c>
-      <c r="B75" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+      <c r="B76" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>131</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
+      <c r="B77" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>132</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+      <c r="B78" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="C78" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>134</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+      <c r="B79" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>135</v>
       </c>
-      <c r="B79" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+      <c r="B80" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="C80" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="7" t="s">
+      <c r="B81" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B81" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="7" t="s">
+      <c r="B82" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="C82" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>140</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
+      <c r="B83" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>141</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
+      <c r="B84" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>142</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
+      <c r="B85" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="C85" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>144</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
+      <c r="B86" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>145</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+      <c r="B87" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>146</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
+      <c r="B88" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="C88" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>148</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
+      <c r="B89" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>149</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+      <c r="B90" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>150</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+      <c r="B91" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="C91" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>152</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>153</v>
-      </c>
       <c r="B92" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>153</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="C93" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C93" s="3" t="s">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
+      <c r="B94" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>157</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
+      <c r="B95" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>158</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
+      <c r="B96" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="C96" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>160</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>161</v>
-      </c>
       <c r="B97" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>162</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
+      <c r="B99" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>165</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>166</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
+      <c r="B102" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>171</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>174</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>175</v>
       </c>
-      <c r="B108" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
+      <c r="B109" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>177</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>178</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
+        <v>181</v>
+      </c>
+      <c r="B113" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>183</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B114" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C114" s="3" t="s">
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
+      <c r="B115" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>186</v>
       </c>
-      <c r="B115" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
+      <c r="B116" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>9</v>

</xml_diff>